<commit_message>
added stuff, mostly worked on insert text and added getnextemptycell
</commit_message>
<xml_diff>
--- a/COMP72070_Section3_Group1/testexcel.xlsx
+++ b/COMP72070_Section3_Group1/testexcel.xlsx
@@ -8,17 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\source\repos\proj 4\COMP72070_Section3_Group1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE6733E-FB0C-4D70-A4D1-F7873BF7870F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C970D062-5A27-43F8-99D3-59325308C74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,35 +25,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
-  <si>
-    <t>hello world</t>
-  </si>
-  <si>
-    <t>what 1</t>
-  </si>
-  <si>
-    <t>line 3?</t>
-  </si>
-  <si>
-    <t>TimeStamp</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>5:03:00PM July 27th 2024</t>
-  </si>
-  <si>
-    <t>Yao</t>
-  </si>
-  <si>
-    <t>Tried to hack into the system and failed</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+  <x:si>
+    <x:t>TimeStamp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>User</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Action</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5:03:00PM July 27th 2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Yao</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tried to hack into the system and failed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12:53:30AM April 16th 2021</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,127 +362,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:dimension ref="A1:C7"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="C10" sqref="C10"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:cols>
+    <x:col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="4.77734375" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="33.44140625" bestFit="1" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3">
+      <x:c r="A3" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</x:worksheet>
 </file>
</xml_diff>